<commit_message>
přejmenovávání a finální úpravy
</commit_message>
<xml_diff>
--- a/ADC korekce.xlsx
+++ b/ADC korekce.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mechatronika\zdroj\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F423C6A9-3573-49A9-A01B-45B59CF653E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE92C039-65CF-417A-8F42-D7B673CE690D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{701769E6-910C-495F-9108-E9F7473121A3}"/>
   </bookViews>
@@ -80,7 +80,7 @@
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -307,10 +307,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -1923,16 +1923,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>395654</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>188589</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>80962</xdr:rowOff>
+      <xdr:rowOff>31266</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>154886</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>45554</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2259,8 +2259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6E353EB-305F-4836-8586-AFDB78AFBECF}">
   <dimension ref="A7:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I42" sqref="B8:I42"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>